<commit_message>
Changed directory structure and updated navbar links
</commit_message>
<xml_diff>
--- a/Documents/Plan.xlsx
+++ b/Documents/Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\wigglememore3d\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PersonalRepos\wigglememore3d\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072D056E-532E-45A4-88C2-F28A382E80F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF081758-E4E1-47E9-86AC-764492393E5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -507,18 +507,18 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -532,12 +532,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -548,27 +548,27 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>33</v>
       </c>
@@ -576,7 +576,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>35</v>
       </c>
@@ -587,17 +587,17 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -608,12 +608,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>42</v>
       </c>
@@ -621,12 +621,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>23</v>
       </c>
@@ -634,12 +634,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>24</v>
       </c>
@@ -647,12 +647,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>25</v>
       </c>
@@ -660,12 +660,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>43</v>
       </c>
@@ -673,12 +673,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -689,57 +689,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>3</v>
       </c>
@@ -747,12 +747,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>44</v>
       </c>
@@ -760,22 +760,22 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>4</v>
       </c>
@@ -783,12 +783,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Update html pages, navbar correct on all, started logo design
</commit_message>
<xml_diff>
--- a/Documents/Plan.xlsx
+++ b/Documents/Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PersonalRepos\wigglememore3d\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF081758-E4E1-47E9-86AC-764492393E5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91639C3F-B399-46F0-BC09-6F80D9CC2B30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -506,14 +506,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Updated plan, added Marlin guide page and updated all nav-bar links
</commit_message>
<xml_diff>
--- a/Documents/Plan.xlsx
+++ b/Documents/Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PersonalRepos\wigglememore3d\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\wigglememore3d\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370B5733-2FC4-4BE5-87FA-FCCA2E17F768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4752C19-C9DD-4D80-90A5-FAFC2B4A0264}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,23 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>Home</t>
   </si>
   <si>
-    <t>Modifications</t>
-  </si>
-  <si>
-    <t>Printable</t>
-  </si>
-  <si>
-    <t>Hardware</t>
-  </si>
-  <si>
-    <t>Electronics</t>
-  </si>
-  <si>
     <t>Bed supports</t>
   </si>
   <si>
@@ -189,13 +177,28 @@
     <t>Marlin</t>
   </si>
   <si>
-    <t>My Ender 5 Journey</t>
-  </si>
-  <si>
     <t>About Me</t>
   </si>
   <si>
     <t>Contact</t>
+  </si>
+  <si>
+    <t>Guides</t>
+  </si>
+  <si>
+    <t>Ender 5</t>
+  </si>
+  <si>
+    <t>Journey</t>
+  </si>
+  <si>
+    <t>Printable mods</t>
+  </si>
+  <si>
+    <t>Hardware mods</t>
+  </si>
+  <si>
+    <t>Electronics mods</t>
   </si>
 </sst>
 </file>
@@ -513,36 +516,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -550,278 +553,283 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>52</v>
-      </c>
-      <c r="D44" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>